<commit_message>
NN, NO and CSV
</commit_message>
<xml_diff>
--- a/data/brainPeps..xlsx
+++ b/data/brainPeps..xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="125">
   <si>
     <t xml:space="preserve">onelettersequence</t>
   </si>
@@ -217,16 +217,13 @@
     <t xml:space="preserve">GSS(octanoyl)FLSPEHQKAQQRKESKKPPAKLQPR</t>
   </si>
   <si>
-    <t xml:space="preserve">(2'-N-succinimide-paclitaxel)TFFYGGSRG-(2'-N-succinimide-paclitaxel)KRNNF(2'-N-succinimide-paclitaxel)KTEEY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Benzylpenicillin-RGGRLSYSRRRFSTSTGR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doxorubicin-linker-RGGRLSYSRRRFSTSTGR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Doxorubicin-linker-RRLSYSRRRF</t>
+    <t xml:space="preserve">TFFYGGSRG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGGRLSYSRRRFSTSTGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RRLSYSRRRF</t>
   </si>
   <si>
     <t xml:space="preserve">YWAGGDASGE</t>
@@ -235,10 +232,10 @@
     <t xml:space="preserve">NA</t>
   </si>
   <si>
-    <t xml:space="preserve">YPLG-NH&lt;sub&gt;2&lt;/sub&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLG-NH&lt;sub&gt;2&lt;/sub&gt;</t>
+    <t xml:space="preserve">YPLG-NH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLG-NH</t>
   </si>
   <si>
     <t xml:space="preserve">DAEFRHDSGYQVHHQKLVFFAEDVGSNK</t>
@@ -247,7 +244,7 @@
     <t xml:space="preserve">DAEFRHDSGYEVHHQKLVFFAEDVGSNKGAIIGLMVGGVV</t>
   </si>
   <si>
-    <t xml:space="preserve">YPFP-NH&lt;sub&gt;2&lt;/sub&gt;</t>
+    <t xml:space="preserve">YPFP-NH</t>
   </si>
   <si>
     <t xml:space="preserve">CKGKGAKCSRLMYDCCTGSCRSGKC</t>
@@ -373,7 +370,7 @@
     <t xml:space="preserve">CGGKTFFYGGSRGKRNNFKTEEY</t>
   </si>
   <si>
-    <t xml:space="preserve">long unstructured flexible chain: HKKWQFNSPFVPRADEPARKGKVHIPFPLDNITC rigid β-hairpin structure: RVPMAREPTVIHGKREVTLHLHPDH</t>
+    <t xml:space="preserve">HKKWQFNSPFVPRADEPARKGKVHIPFPLDNITC</t>
   </si>
   <si>
     <t xml:space="preserve">GLHTSATNLYLH</t>
@@ -416,7 +413,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -452,6 +449,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -503,7 +506,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -520,7 +523,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -603,11 +614,11 @@
   </sheetPr>
   <dimension ref="A1:A130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A80" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A92" activeCellId="0" sqref="A92"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -924,29 +935,29 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="2" t="s">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -956,202 +967,202 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,102 +1172,102 @@
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="4" t="s">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="4" t="s">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="4" t="s">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="6" t="s">
         <v>117</v>
-      </c>
-    </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>